<commit_message>
chore: bump assets v=20251104_155956
Signed-off-by: nataliohoteles-crypto <comunicaciones@hotelguadiana.es>
</commit_message>
<xml_diff>
--- a/plantilla_preguntas_unica.xlsx
+++ b/plantilla_preguntas_unica.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7cdc5f6b199a606e/02. Comp. Min Recepción/Web Test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comun\Documents\Web Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="272" documentId="11_A3A8323C874F6E2F9F9036ABEDF7ECD0F4240C3C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7703FD8C-615E-46D6-BCAF-AB4C73AC309B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DA2F58-EB2D-41E1-9A24-A51D2F4C3942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27840" yWindow="960" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Preguntas" sheetId="2" r:id="rId1"/>
@@ -2591,9 +2591,6 @@
     <t>DTO</t>
   </si>
   <si>
-    <t>Recepcióon</t>
-  </si>
-  <si>
     <t>¿Cuál es el riesgo principal de modificar el localizador antes de que sincronice el channel manager?</t>
   </si>
   <si>
@@ -3129,6 +3126,9 @@
   </si>
   <si>
     <t>Errores Comunes</t>
+  </si>
+  <si>
+    <t>Recepción</t>
   </si>
 </sst>
 </file>
@@ -4151,8 +4151,8 @@
   <dimension ref="A1:M182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E174" sqref="E174"/>
+      <pane ySplit="1" topLeftCell="A181" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D188" sqref="D188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4214,7 +4214,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>12</v>
@@ -4256,7 +4256,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
@@ -4298,7 +4298,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>12</v>
@@ -4340,7 +4340,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>12</v>
@@ -4382,7 +4382,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>12</v>
@@ -4424,7 +4424,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>12</v>
@@ -4466,7 +4466,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>12</v>
@@ -4508,7 +4508,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>12</v>
@@ -4550,7 +4550,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>12</v>
@@ -4592,7 +4592,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>12</v>
@@ -4634,7 +4634,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>12</v>
@@ -4676,7 +4676,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>12</v>
@@ -4718,7 +4718,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>12</v>
@@ -4760,7 +4760,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>12</v>
@@ -4802,7 +4802,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>12</v>
@@ -4844,7 +4844,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>12</v>
@@ -4886,7 +4886,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>12</v>
@@ -4928,7 +4928,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>12</v>
@@ -4970,7 +4970,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>12</v>
@@ -5012,7 +5012,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>12</v>
@@ -5054,7 +5054,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>12</v>
@@ -5096,7 +5096,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>12</v>
@@ -5138,7 +5138,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>12</v>
@@ -5180,7 +5180,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>12</v>
@@ -5222,7 +5222,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>12</v>
@@ -5264,7 +5264,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>12</v>
@@ -5306,7 +5306,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>12</v>
@@ -5348,7 +5348,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>12</v>
@@ -5390,7 +5390,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>12</v>
@@ -5432,7 +5432,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>12</v>
@@ -5474,7 +5474,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>12</v>
@@ -5516,7 +5516,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>12</v>
@@ -5558,7 +5558,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>12</v>
@@ -5600,7 +5600,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>12</v>
@@ -5642,7 +5642,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>12</v>
@@ -5684,7 +5684,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>12</v>
@@ -5726,7 +5726,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>12</v>
@@ -5768,7 +5768,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>12</v>
@@ -5810,7 +5810,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>12</v>
@@ -5852,7 +5852,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>12</v>
@@ -5894,7 +5894,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>12</v>
@@ -5936,7 +5936,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>12</v>
@@ -5978,7 +5978,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>12</v>
@@ -6020,7 +6020,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>12</v>
@@ -6062,7 +6062,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>12</v>
@@ -6104,7 +6104,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>12</v>
@@ -6146,7 +6146,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>12</v>
@@ -6188,7 +6188,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>12</v>
@@ -6230,7 +6230,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>12</v>
@@ -6272,7 +6272,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>12</v>
@@ -6314,7 +6314,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>12</v>
@@ -6356,7 +6356,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>12</v>
@@ -6398,7 +6398,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>12</v>
@@ -6440,7 +6440,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>12</v>
@@ -6482,7 +6482,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>12</v>
@@ -6524,7 +6524,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>12</v>
@@ -6566,7 +6566,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>12</v>
@@ -6608,7 +6608,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>12</v>
@@ -6650,7 +6650,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>12</v>
@@ -6692,7 +6692,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>12</v>
@@ -6734,7 +6734,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>12</v>
@@ -6776,7 +6776,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>12</v>
@@ -6818,7 +6818,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>12</v>
@@ -6860,7 +6860,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>12</v>
@@ -6902,7 +6902,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>12</v>
@@ -6944,7 +6944,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>12</v>
@@ -6986,7 +6986,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>12</v>
@@ -7028,7 +7028,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>12</v>
@@ -7070,7 +7070,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>12</v>
@@ -7112,7 +7112,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>12</v>
@@ -7154,7 +7154,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>12</v>
@@ -7196,7 +7196,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>12</v>
@@ -7238,7 +7238,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>12</v>
@@ -7280,7 +7280,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>12</v>
@@ -7322,7 +7322,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>12</v>
@@ -7364,7 +7364,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>402</v>
@@ -7406,7 +7406,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>402</v>
@@ -7448,7 +7448,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>402</v>
@@ -7490,7 +7490,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>402</v>
@@ -7532,7 +7532,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>402</v>
@@ -7574,7 +7574,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>402</v>
@@ -7616,7 +7616,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>402</v>
@@ -7658,7 +7658,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>402</v>
@@ -7700,7 +7700,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>402</v>
@@ -7742,7 +7742,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>402</v>
@@ -7784,7 +7784,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C87" s="5" t="s">
         <v>402</v>
@@ -7826,7 +7826,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C88" s="5" t="s">
         <v>402</v>
@@ -7868,7 +7868,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>402</v>
@@ -7910,7 +7910,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>402</v>
@@ -7952,7 +7952,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>402</v>
@@ -7994,7 +7994,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C92" s="5" t="s">
         <v>402</v>
@@ -8036,7 +8036,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C93" s="5" t="s">
         <v>402</v>
@@ -8078,7 +8078,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>402</v>
@@ -8120,7 +8120,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>402</v>
@@ -8162,7 +8162,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>402</v>
@@ -8204,7 +8204,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>402</v>
@@ -8246,7 +8246,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>402</v>
@@ -8288,7 +8288,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>402</v>
@@ -8330,7 +8330,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>402</v>
@@ -8372,7 +8372,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>402</v>
@@ -8414,7 +8414,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>402</v>
@@ -8456,7 +8456,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>402</v>
@@ -8498,7 +8498,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>402</v>
@@ -8540,7 +8540,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>402</v>
@@ -8582,7 +8582,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>402</v>
@@ -8624,7 +8624,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C107" s="5" t="s">
         <v>402</v>
@@ -8666,7 +8666,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C108" s="5" t="s">
         <v>402</v>
@@ -8708,7 +8708,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C109" s="5" t="s">
         <v>402</v>
@@ -8750,7 +8750,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C110" s="5" t="s">
         <v>402</v>
@@ -8792,7 +8792,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C111" s="5" t="s">
         <v>402</v>
@@ -8834,7 +8834,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C112" s="5" t="s">
         <v>402</v>
@@ -8876,7 +8876,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C113" s="5" t="s">
         <v>402</v>
@@ -8918,7 +8918,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C114" s="5" t="s">
         <v>402</v>
@@ -8960,7 +8960,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C115" s="5" t="s">
         <v>402</v>
@@ -9002,7 +9002,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C116" s="5" t="s">
         <v>402</v>
@@ -9044,7 +9044,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C117" s="5" t="s">
         <v>402</v>
@@ -9086,7 +9086,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C118" s="5" t="s">
         <v>402</v>
@@ -9128,7 +9128,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C119" s="5" t="s">
         <v>402</v>
@@ -9170,7 +9170,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C120" s="5" t="s">
         <v>402</v>
@@ -9212,7 +9212,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C121" s="5" t="s">
         <v>402</v>
@@ -9254,7 +9254,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C122" s="5" t="s">
         <v>402</v>
@@ -9296,7 +9296,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C123" s="5" t="s">
         <v>402</v>
@@ -9338,7 +9338,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C124" s="5" t="s">
         <v>402</v>
@@ -9380,7 +9380,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C125" s="5" t="s">
         <v>402</v>
@@ -9422,7 +9422,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C126" s="5" t="s">
         <v>402</v>
@@ -9464,7 +9464,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C127" s="5" t="s">
         <v>402</v>
@@ -9506,7 +9506,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C128" s="5" t="s">
         <v>402</v>
@@ -9548,7 +9548,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C129" s="5" t="s">
         <v>402</v>
@@ -9590,7 +9590,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C130" s="5" t="s">
         <v>402</v>
@@ -9632,7 +9632,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C131" s="5" t="s">
         <v>402</v>
@@ -9674,7 +9674,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C132" s="5" t="s">
         <v>402</v>
@@ -9716,7 +9716,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C133" s="5" t="s">
         <v>402</v>
@@ -9758,7 +9758,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C134" s="5" t="s">
         <v>402</v>
@@ -9800,7 +9800,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C135" s="5" t="s">
         <v>402</v>
@@ -9842,7 +9842,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C136" s="5" t="s">
         <v>402</v>
@@ -9884,7 +9884,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C137" s="5" t="s">
         <v>402</v>
@@ -9926,7 +9926,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C138" s="5" t="s">
         <v>402</v>
@@ -9968,7 +9968,7 @@
         <v>138</v>
       </c>
       <c r="B139" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C139" s="5" t="s">
         <v>402</v>
@@ -10010,7 +10010,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C140" s="5" t="s">
         <v>402</v>
@@ -10052,7 +10052,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C141" s="5" t="s">
         <v>402</v>
@@ -10094,7 +10094,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C142" s="5" t="s">
         <v>402</v>
@@ -10136,7 +10136,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C143" s="5" t="s">
         <v>402</v>
@@ -10178,7 +10178,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C144" s="5" t="s">
         <v>402</v>
@@ -10220,7 +10220,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C145" s="5" t="s">
         <v>402</v>
@@ -10262,7 +10262,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C146" s="5" t="s">
         <v>402</v>
@@ -10304,7 +10304,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C147" s="5" t="s">
         <v>402</v>
@@ -10346,7 +10346,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C148" s="5" t="s">
         <v>402</v>
@@ -10388,7 +10388,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C149" s="5" t="s">
         <v>402</v>
@@ -10430,7 +10430,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C150" s="5" t="s">
         <v>402</v>
@@ -10472,7 +10472,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C151" s="5" t="s">
         <v>402</v>
@@ -10514,7 +10514,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C152" s="5" t="s">
         <v>402</v>
@@ -10556,28 +10556,28 @@
         <v>152</v>
       </c>
       <c r="B153" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D153" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E153" s="19" t="s">
+        <v>851</v>
+      </c>
+      <c r="F153" s="19" t="s">
         <v>852</v>
       </c>
-      <c r="F153" s="19" t="s">
+      <c r="G153" s="19" t="s">
         <v>853</v>
       </c>
-      <c r="G153" s="19" t="s">
+      <c r="H153" s="19" t="s">
         <v>854</v>
       </c>
-      <c r="H153" s="19" t="s">
+      <c r="I153" s="19" t="s">
         <v>855</v>
-      </c>
-      <c r="I153" s="19" t="s">
-        <v>856</v>
       </c>
       <c r="J153" s="17" t="s">
         <v>5</v>
@@ -10587,7 +10587,7 @@
         <v>B</v>
       </c>
       <c r="L153" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="M153" s="9">
         <v>1</v>
@@ -10598,28 +10598,28 @@
         <v>153</v>
       </c>
       <c r="B154" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D154" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E154" s="19" t="s">
+        <v>856</v>
+      </c>
+      <c r="F154" s="19" t="s">
         <v>857</v>
       </c>
-      <c r="F154" s="19" t="s">
+      <c r="G154" s="19" t="s">
         <v>858</v>
       </c>
-      <c r="G154" s="19" t="s">
+      <c r="H154" s="19" t="s">
         <v>859</v>
       </c>
-      <c r="H154" s="19" t="s">
+      <c r="I154" s="19" t="s">
         <v>860</v>
-      </c>
-      <c r="I154" s="19" t="s">
-        <v>861</v>
       </c>
       <c r="J154" s="17" t="s">
         <v>6</v>
@@ -10629,7 +10629,7 @@
         <v>C</v>
       </c>
       <c r="L154" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="M154" s="9">
         <v>1</v>
@@ -10640,28 +10640,28 @@
         <v>154</v>
       </c>
       <c r="B155" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D155" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E155" s="19" t="s">
+        <v>861</v>
+      </c>
+      <c r="F155" s="19" t="s">
         <v>862</v>
       </c>
-      <c r="F155" s="19" t="s">
+      <c r="G155" s="19" t="s">
         <v>863</v>
       </c>
-      <c r="G155" s="19" t="s">
+      <c r="H155" s="19" t="s">
         <v>864</v>
       </c>
-      <c r="H155" s="19" t="s">
+      <c r="I155" s="19" t="s">
         <v>865</v>
-      </c>
-      <c r="I155" s="19" t="s">
-        <v>866</v>
       </c>
       <c r="J155" s="17" t="s">
         <v>5</v>
@@ -10671,7 +10671,7 @@
         <v>B</v>
       </c>
       <c r="L155" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="M155" s="9">
         <v>1</v>
@@ -10682,28 +10682,28 @@
         <v>155</v>
       </c>
       <c r="B156" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D156" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E156" s="19" t="s">
+        <v>866</v>
+      </c>
+      <c r="F156" s="19" t="s">
         <v>867</v>
       </c>
-      <c r="F156" s="19" t="s">
+      <c r="G156" s="19" t="s">
         <v>868</v>
       </c>
-      <c r="G156" s="19" t="s">
+      <c r="H156" s="19" t="s">
         <v>869</v>
       </c>
-      <c r="H156" s="19" t="s">
+      <c r="I156" s="19" t="s">
         <v>870</v>
-      </c>
-      <c r="I156" s="19" t="s">
-        <v>871</v>
       </c>
       <c r="J156" s="17" t="s">
         <v>5</v>
@@ -10713,7 +10713,7 @@
         <v>B</v>
       </c>
       <c r="L156" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="M156" s="9">
         <v>1</v>
@@ -10724,28 +10724,28 @@
         <v>156</v>
       </c>
       <c r="B157" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D157" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E157" s="19" t="s">
+        <v>871</v>
+      </c>
+      <c r="F157" s="19" t="s">
         <v>872</v>
       </c>
-      <c r="F157" s="19" t="s">
+      <c r="G157" s="19" t="s">
         <v>873</v>
       </c>
-      <c r="G157" s="19" t="s">
+      <c r="H157" s="19" t="s">
         <v>874</v>
       </c>
-      <c r="H157" s="19" t="s">
+      <c r="I157" s="19" t="s">
         <v>875</v>
-      </c>
-      <c r="I157" s="19" t="s">
-        <v>876</v>
       </c>
       <c r="J157" s="17" t="s">
         <v>5</v>
@@ -10755,7 +10755,7 @@
         <v>B</v>
       </c>
       <c r="L157" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="M157" s="9">
         <v>1</v>
@@ -10766,28 +10766,28 @@
         <v>157</v>
       </c>
       <c r="B158" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D158" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E158" s="19" t="s">
+        <v>876</v>
+      </c>
+      <c r="F158" s="19" t="s">
         <v>877</v>
       </c>
-      <c r="F158" s="19" t="s">
+      <c r="G158" s="19" t="s">
         <v>878</v>
       </c>
-      <c r="G158" s="19" t="s">
+      <c r="H158" s="19" t="s">
         <v>879</v>
       </c>
-      <c r="H158" s="19" t="s">
+      <c r="I158" s="19" t="s">
         <v>880</v>
-      </c>
-      <c r="I158" s="19" t="s">
-        <v>881</v>
       </c>
       <c r="J158" s="17" t="s">
         <v>5</v>
@@ -10797,7 +10797,7 @@
         <v>B</v>
       </c>
       <c r="L158" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="M158" s="9">
         <v>1</v>
@@ -10808,25 +10808,25 @@
         <v>158</v>
       </c>
       <c r="B159" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D159" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E159" s="19" t="s">
+        <v>881</v>
+      </c>
+      <c r="F159" s="19" t="s">
         <v>882</v>
       </c>
-      <c r="F159" s="19" t="s">
+      <c r="G159" s="19" t="s">
         <v>883</v>
       </c>
-      <c r="G159" s="19" t="s">
+      <c r="H159" s="19" t="s">
         <v>884</v>
-      </c>
-      <c r="H159" s="19" t="s">
-        <v>885</v>
       </c>
       <c r="I159" s="19" t="s">
         <v>424</v>
@@ -10839,7 +10839,7 @@
         <v>B</v>
       </c>
       <c r="L159" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="M159" s="9">
         <v>1</v>
@@ -10850,28 +10850,28 @@
         <v>159</v>
       </c>
       <c r="B160" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D160" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E160" s="19" t="s">
+        <v>885</v>
+      </c>
+      <c r="F160" s="19" t="s">
         <v>886</v>
       </c>
-      <c r="F160" s="19" t="s">
+      <c r="G160" s="19" t="s">
         <v>887</v>
       </c>
-      <c r="G160" s="19" t="s">
+      <c r="H160" s="19" t="s">
         <v>888</v>
       </c>
-      <c r="H160" s="19" t="s">
+      <c r="I160" s="19" t="s">
         <v>889</v>
-      </c>
-      <c r="I160" s="19" t="s">
-        <v>890</v>
       </c>
       <c r="J160" s="17" t="s">
         <v>5</v>
@@ -10881,7 +10881,7 @@
         <v>B</v>
       </c>
       <c r="L160" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="M160" s="9">
         <v>1</v>
@@ -10892,28 +10892,28 @@
         <v>160</v>
       </c>
       <c r="B161" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D161" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E161" s="19" t="s">
+        <v>890</v>
+      </c>
+      <c r="F161" s="19" t="s">
         <v>891</v>
       </c>
-      <c r="F161" s="19" t="s">
+      <c r="G161" s="19" t="s">
         <v>892</v>
       </c>
-      <c r="G161" s="19" t="s">
+      <c r="H161" s="19" t="s">
         <v>893</v>
       </c>
-      <c r="H161" s="19" t="s">
+      <c r="I161" s="19" t="s">
         <v>894</v>
-      </c>
-      <c r="I161" s="19" t="s">
-        <v>895</v>
       </c>
       <c r="J161" s="17" t="s">
         <v>5</v>
@@ -10923,7 +10923,7 @@
         <v>B</v>
       </c>
       <c r="L161" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="M161" s="9">
         <v>1</v>
@@ -10934,28 +10934,28 @@
         <v>161</v>
       </c>
       <c r="B162" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D162" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E162" s="19" t="s">
+        <v>895</v>
+      </c>
+      <c r="F162" s="19" t="s">
         <v>896</v>
       </c>
-      <c r="F162" s="19" t="s">
+      <c r="G162" s="19" t="s">
         <v>897</v>
       </c>
-      <c r="G162" s="19" t="s">
+      <c r="H162" s="19" t="s">
         <v>898</v>
       </c>
-      <c r="H162" s="19" t="s">
+      <c r="I162" s="19" t="s">
         <v>899</v>
-      </c>
-      <c r="I162" s="19" t="s">
-        <v>900</v>
       </c>
       <c r="J162" s="17" t="s">
         <v>5</v>
@@ -10965,7 +10965,7 @@
         <v>B</v>
       </c>
       <c r="L162" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="M162" s="9">
         <v>1</v>
@@ -10976,28 +10976,28 @@
         <v>162</v>
       </c>
       <c r="B163" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D163" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E163" s="19" t="s">
+        <v>900</v>
+      </c>
+      <c r="F163" s="19" t="s">
         <v>901</v>
       </c>
-      <c r="F163" s="19" t="s">
+      <c r="G163" s="19" t="s">
         <v>902</v>
       </c>
-      <c r="G163" s="19" t="s">
+      <c r="H163" s="19" t="s">
         <v>903</v>
       </c>
-      <c r="H163" s="19" t="s">
+      <c r="I163" s="19" t="s">
         <v>904</v>
-      </c>
-      <c r="I163" s="19" t="s">
-        <v>905</v>
       </c>
       <c r="J163" s="17" t="s">
         <v>5</v>
@@ -11007,7 +11007,7 @@
         <v>B</v>
       </c>
       <c r="L163" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="M163" s="9">
         <v>1</v>
@@ -11018,28 +11018,28 @@
         <v>163</v>
       </c>
       <c r="B164" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D164" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E164" s="19" t="s">
+        <v>905</v>
+      </c>
+      <c r="F164" s="19" t="s">
         <v>906</v>
       </c>
-      <c r="F164" s="19" t="s">
+      <c r="G164" s="19" t="s">
         <v>907</v>
       </c>
-      <c r="G164" s="19" t="s">
+      <c r="H164" s="19" t="s">
         <v>908</v>
       </c>
-      <c r="H164" s="19" t="s">
+      <c r="I164" s="19" t="s">
         <v>909</v>
-      </c>
-      <c r="I164" s="19" t="s">
-        <v>910</v>
       </c>
       <c r="J164" s="17" t="s">
         <v>5</v>
@@ -11049,7 +11049,7 @@
         <v>B</v>
       </c>
       <c r="L164" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="M164" s="9">
         <v>1</v>
@@ -11060,28 +11060,28 @@
         <v>164</v>
       </c>
       <c r="B165" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D165" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E165" s="19" t="s">
+        <v>910</v>
+      </c>
+      <c r="F165" s="19" t="s">
         <v>911</v>
       </c>
-      <c r="F165" s="19" t="s">
+      <c r="G165" s="19" t="s">
         <v>912</v>
       </c>
-      <c r="G165" s="19" t="s">
+      <c r="H165" s="19" t="s">
         <v>913</v>
       </c>
-      <c r="H165" s="19" t="s">
+      <c r="I165" s="19" t="s">
         <v>914</v>
-      </c>
-      <c r="I165" s="19" t="s">
-        <v>915</v>
       </c>
       <c r="J165" s="17" t="s">
         <v>5</v>
@@ -11091,7 +11091,7 @@
         <v>B</v>
       </c>
       <c r="L165" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="M165" s="9">
         <v>1</v>
@@ -11102,28 +11102,28 @@
         <v>165</v>
       </c>
       <c r="B166" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D166" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E166" s="19" t="s">
+        <v>915</v>
+      </c>
+      <c r="F166" s="19" t="s">
         <v>916</v>
       </c>
-      <c r="F166" s="19" t="s">
+      <c r="G166" s="19" t="s">
         <v>917</v>
       </c>
-      <c r="G166" s="19" t="s">
+      <c r="H166" s="19" t="s">
         <v>918</v>
       </c>
-      <c r="H166" s="19" t="s">
+      <c r="I166" s="19" t="s">
         <v>919</v>
-      </c>
-      <c r="I166" s="19" t="s">
-        <v>920</v>
       </c>
       <c r="J166" s="17" t="s">
         <v>5</v>
@@ -11133,7 +11133,7 @@
         <v>B</v>
       </c>
       <c r="L166" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="M166" s="9">
         <v>1</v>
@@ -11144,28 +11144,28 @@
         <v>166</v>
       </c>
       <c r="B167" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D167" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E167" s="19" t="s">
+        <v>920</v>
+      </c>
+      <c r="F167" s="19" t="s">
         <v>921</v>
       </c>
-      <c r="F167" s="19" t="s">
+      <c r="G167" s="19" t="s">
         <v>922</v>
       </c>
-      <c r="G167" s="19" t="s">
+      <c r="H167" s="19" t="s">
         <v>923</v>
       </c>
-      <c r="H167" s="19" t="s">
+      <c r="I167" s="19" t="s">
         <v>924</v>
-      </c>
-      <c r="I167" s="19" t="s">
-        <v>925</v>
       </c>
       <c r="J167" s="17" t="s">
         <v>5</v>
@@ -11175,7 +11175,7 @@
         <v>B</v>
       </c>
       <c r="L167" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="M167" s="9">
         <v>1</v>
@@ -11186,28 +11186,28 @@
         <v>167</v>
       </c>
       <c r="B168" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D168" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E168" s="19" t="s">
+        <v>925</v>
+      </c>
+      <c r="F168" s="19" t="s">
         <v>926</v>
       </c>
-      <c r="F168" s="19" t="s">
+      <c r="G168" s="19" t="s">
         <v>927</v>
       </c>
-      <c r="G168" s="19" t="s">
+      <c r="H168" s="19" t="s">
         <v>928</v>
       </c>
-      <c r="H168" s="19" t="s">
+      <c r="I168" s="19" t="s">
         <v>929</v>
-      </c>
-      <c r="I168" s="19" t="s">
-        <v>930</v>
       </c>
       <c r="J168" s="17" t="s">
         <v>5</v>
@@ -11217,7 +11217,7 @@
         <v>B</v>
       </c>
       <c r="L168" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="M168" s="9">
         <v>1</v>
@@ -11228,28 +11228,28 @@
         <v>168</v>
       </c>
       <c r="B169" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D169" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E169" s="19" t="s">
+        <v>930</v>
+      </c>
+      <c r="F169" s="19" t="s">
         <v>931</v>
       </c>
-      <c r="F169" s="19" t="s">
+      <c r="G169" s="19" t="s">
         <v>932</v>
       </c>
-      <c r="G169" s="19" t="s">
+      <c r="H169" s="19" t="s">
         <v>933</v>
       </c>
-      <c r="H169" s="19" t="s">
+      <c r="I169" s="19" t="s">
         <v>934</v>
-      </c>
-      <c r="I169" s="19" t="s">
-        <v>935</v>
       </c>
       <c r="J169" s="17" t="s">
         <v>5</v>
@@ -11259,7 +11259,7 @@
         <v>B</v>
       </c>
       <c r="L169" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="M169" s="9">
         <v>1</v>
@@ -11270,28 +11270,28 @@
         <v>169</v>
       </c>
       <c r="B170" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D170" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E170" s="19" t="s">
+        <v>935</v>
+      </c>
+      <c r="F170" s="19" t="s">
         <v>936</v>
       </c>
-      <c r="F170" s="19" t="s">
+      <c r="G170" s="19" t="s">
         <v>937</v>
       </c>
-      <c r="G170" s="19" t="s">
+      <c r="H170" s="19" t="s">
         <v>938</v>
       </c>
-      <c r="H170" s="19" t="s">
+      <c r="I170" s="19" t="s">
         <v>939</v>
-      </c>
-      <c r="I170" s="19" t="s">
-        <v>940</v>
       </c>
       <c r="J170" s="17" t="s">
         <v>5</v>
@@ -11301,7 +11301,7 @@
         <v>B</v>
       </c>
       <c r="L170" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="M170" s="9">
         <v>1</v>
@@ -11312,28 +11312,28 @@
         <v>170</v>
       </c>
       <c r="B171" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D171" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E171" s="19" t="s">
+        <v>940</v>
+      </c>
+      <c r="F171" s="19" t="s">
         <v>941</v>
       </c>
-      <c r="F171" s="19" t="s">
+      <c r="G171" s="19" t="s">
         <v>942</v>
       </c>
-      <c r="G171" s="19" t="s">
+      <c r="H171" s="19" t="s">
         <v>943</v>
       </c>
-      <c r="H171" s="19" t="s">
+      <c r="I171" s="19" t="s">
         <v>944</v>
-      </c>
-      <c r="I171" s="19" t="s">
-        <v>945</v>
       </c>
       <c r="J171" s="17" t="s">
         <v>5</v>
@@ -11343,7 +11343,7 @@
         <v>B</v>
       </c>
       <c r="L171" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="M171" s="9">
         <v>1</v>
@@ -11354,28 +11354,28 @@
         <v>171</v>
       </c>
       <c r="B172" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D172" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E172" s="19" t="s">
+        <v>945</v>
+      </c>
+      <c r="F172" s="19" t="s">
         <v>946</v>
       </c>
-      <c r="F172" s="19" t="s">
+      <c r="G172" s="19" t="s">
         <v>947</v>
       </c>
-      <c r="G172" s="19" t="s">
+      <c r="H172" s="19" t="s">
         <v>948</v>
       </c>
-      <c r="H172" s="19" t="s">
+      <c r="I172" s="19" t="s">
         <v>949</v>
-      </c>
-      <c r="I172" s="19" t="s">
-        <v>950</v>
       </c>
       <c r="J172" s="17" t="s">
         <v>5</v>
@@ -11385,7 +11385,7 @@
         <v>B</v>
       </c>
       <c r="L172" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="M172" s="9">
         <v>1</v>
@@ -11396,28 +11396,28 @@
         <v>172</v>
       </c>
       <c r="B173" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D173" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E173" s="19" t="s">
+        <v>950</v>
+      </c>
+      <c r="F173" s="19" t="s">
         <v>951</v>
       </c>
-      <c r="F173" s="19" t="s">
+      <c r="G173" s="19" t="s">
         <v>952</v>
       </c>
-      <c r="G173" s="19" t="s">
+      <c r="H173" s="19" t="s">
         <v>953</v>
       </c>
-      <c r="H173" s="19" t="s">
+      <c r="I173" s="19" t="s">
         <v>954</v>
-      </c>
-      <c r="I173" s="19" t="s">
-        <v>955</v>
       </c>
       <c r="J173" s="17" t="s">
         <v>5</v>
@@ -11427,7 +11427,7 @@
         <v>B</v>
       </c>
       <c r="L173" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="M173" s="9">
         <v>1</v>
@@ -11438,28 +11438,28 @@
         <v>173</v>
       </c>
       <c r="B174" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C174" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D174" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E174" s="19" t="s">
+        <v>955</v>
+      </c>
+      <c r="F174" s="19" t="s">
         <v>956</v>
       </c>
-      <c r="F174" s="19" t="s">
+      <c r="G174" s="19" t="s">
         <v>957</v>
       </c>
-      <c r="G174" s="19" t="s">
+      <c r="H174" s="19" t="s">
         <v>958</v>
       </c>
-      <c r="H174" s="19" t="s">
+      <c r="I174" s="19" t="s">
         <v>959</v>
-      </c>
-      <c r="I174" s="19" t="s">
-        <v>960</v>
       </c>
       <c r="J174" s="17" t="s">
         <v>5</v>
@@ -11469,7 +11469,7 @@
         <v>B</v>
       </c>
       <c r="L174" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="M174" s="9">
         <v>1</v>
@@ -11480,28 +11480,28 @@
         <v>174</v>
       </c>
       <c r="B175" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C175" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D175" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E175" s="19" t="s">
+        <v>960</v>
+      </c>
+      <c r="F175" s="19" t="s">
         <v>961</v>
       </c>
-      <c r="F175" s="19" t="s">
+      <c r="G175" s="19" t="s">
         <v>962</v>
       </c>
-      <c r="G175" s="19" t="s">
+      <c r="H175" s="19" t="s">
         <v>963</v>
       </c>
-      <c r="H175" s="19" t="s">
+      <c r="I175" s="19" t="s">
         <v>964</v>
-      </c>
-      <c r="I175" s="19" t="s">
-        <v>965</v>
       </c>
       <c r="J175" s="17" t="s">
         <v>5</v>
@@ -11511,7 +11511,7 @@
         <v>B</v>
       </c>
       <c r="L175" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="M175" s="9">
         <v>1</v>
@@ -11522,28 +11522,28 @@
         <v>175</v>
       </c>
       <c r="B176" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C176" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D176" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E176" s="19" t="s">
+        <v>965</v>
+      </c>
+      <c r="F176" s="19" t="s">
         <v>966</v>
       </c>
-      <c r="F176" s="19" t="s">
+      <c r="G176" s="19" t="s">
         <v>967</v>
       </c>
-      <c r="G176" s="19" t="s">
+      <c r="H176" s="19" t="s">
         <v>968</v>
       </c>
-      <c r="H176" s="19" t="s">
+      <c r="I176" s="19" t="s">
         <v>969</v>
-      </c>
-      <c r="I176" s="19" t="s">
-        <v>970</v>
       </c>
       <c r="J176" s="17" t="s">
         <v>5</v>
@@ -11553,7 +11553,7 @@
         <v>B</v>
       </c>
       <c r="L176" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="M176" s="9">
         <v>1</v>
@@ -11564,28 +11564,28 @@
         <v>176</v>
       </c>
       <c r="B177" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D177" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E177" s="19" t="s">
+        <v>970</v>
+      </c>
+      <c r="F177" s="19" t="s">
         <v>971</v>
       </c>
-      <c r="F177" s="19" t="s">
+      <c r="G177" s="19" t="s">
         <v>972</v>
       </c>
-      <c r="G177" s="19" t="s">
+      <c r="H177" s="19" t="s">
         <v>973</v>
       </c>
-      <c r="H177" s="19" t="s">
+      <c r="I177" s="19" t="s">
         <v>974</v>
-      </c>
-      <c r="I177" s="19" t="s">
-        <v>975</v>
       </c>
       <c r="J177" s="17" t="s">
         <v>5</v>
@@ -11595,7 +11595,7 @@
         <v>B</v>
       </c>
       <c r="L177" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="M177" s="9">
         <v>1</v>
@@ -11606,28 +11606,28 @@
         <v>177</v>
       </c>
       <c r="B178" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D178" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E178" s="19" t="s">
+        <v>975</v>
+      </c>
+      <c r="F178" s="19" t="s">
         <v>976</v>
       </c>
-      <c r="F178" s="19" t="s">
+      <c r="G178" s="19" t="s">
         <v>977</v>
       </c>
-      <c r="G178" s="19" t="s">
+      <c r="H178" s="19" t="s">
         <v>978</v>
       </c>
-      <c r="H178" s="19" t="s">
+      <c r="I178" s="19" t="s">
         <v>979</v>
-      </c>
-      <c r="I178" s="19" t="s">
-        <v>980</v>
       </c>
       <c r="J178" s="17" t="s">
         <v>5</v>
@@ -11637,7 +11637,7 @@
         <v>B</v>
       </c>
       <c r="L178" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="M178" s="9">
         <v>1</v>
@@ -11648,28 +11648,28 @@
         <v>178</v>
       </c>
       <c r="B179" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D179" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E179" s="19" t="s">
+        <v>980</v>
+      </c>
+      <c r="F179" s="19" t="s">
         <v>981</v>
       </c>
-      <c r="F179" s="19" t="s">
+      <c r="G179" s="19" t="s">
         <v>982</v>
       </c>
-      <c r="G179" s="19" t="s">
+      <c r="H179" s="19" t="s">
         <v>983</v>
       </c>
-      <c r="H179" s="19" t="s">
+      <c r="I179" s="19" t="s">
         <v>984</v>
-      </c>
-      <c r="I179" s="19" t="s">
-        <v>985</v>
       </c>
       <c r="J179" s="17" t="s">
         <v>5</v>
@@ -11679,7 +11679,7 @@
         <v>B</v>
       </c>
       <c r="L179" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="M179" s="9">
         <v>1</v>
@@ -11690,28 +11690,28 @@
         <v>179</v>
       </c>
       <c r="B180" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C180" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D180" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E180" s="19" t="s">
+        <v>985</v>
+      </c>
+      <c r="F180" s="19" t="s">
         <v>986</v>
       </c>
-      <c r="F180" s="19" t="s">
+      <c r="G180" s="19" t="s">
         <v>987</v>
       </c>
-      <c r="G180" s="19" t="s">
+      <c r="H180" s="19" t="s">
         <v>988</v>
       </c>
-      <c r="H180" s="19" t="s">
+      <c r="I180" s="19" t="s">
         <v>989</v>
-      </c>
-      <c r="I180" s="19" t="s">
-        <v>990</v>
       </c>
       <c r="J180" s="17" t="s">
         <v>5</v>
@@ -11721,7 +11721,7 @@
         <v>B</v>
       </c>
       <c r="L180" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="M180" s="9">
         <v>1</v>
@@ -11732,28 +11732,28 @@
         <v>180</v>
       </c>
       <c r="B181" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C181" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D181" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E181" s="19" t="s">
+        <v>990</v>
+      </c>
+      <c r="F181" s="19" t="s">
         <v>991</v>
       </c>
-      <c r="F181" s="19" t="s">
+      <c r="G181" s="19" t="s">
         <v>992</v>
       </c>
-      <c r="G181" s="19" t="s">
+      <c r="H181" s="19" t="s">
+        <v>903</v>
+      </c>
+      <c r="I181" s="19" t="s">
         <v>993</v>
-      </c>
-      <c r="H181" s="19" t="s">
-        <v>904</v>
-      </c>
-      <c r="I181" s="19" t="s">
-        <v>994</v>
       </c>
       <c r="J181" s="17" t="s">
         <v>5</v>
@@ -11763,7 +11763,7 @@
         <v>B</v>
       </c>
       <c r="L181" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="M181" s="9">
         <v>1</v>
@@ -11774,28 +11774,28 @@
         <v>181</v>
       </c>
       <c r="B182" s="18" t="s">
-        <v>851</v>
+        <v>1030</v>
       </c>
       <c r="C182" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D182" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E182" s="20" t="s">
+        <v>994</v>
+      </c>
+      <c r="F182" s="20" t="s">
         <v>995</v>
       </c>
-      <c r="F182" s="20" t="s">
+      <c r="G182" s="20" t="s">
         <v>996</v>
       </c>
-      <c r="G182" s="20" t="s">
+      <c r="H182" s="20" t="s">
         <v>997</v>
       </c>
-      <c r="H182" s="20" t="s">
+      <c r="I182" s="20" t="s">
         <v>998</v>
-      </c>
-      <c r="I182" s="20" t="s">
-        <v>999</v>
       </c>
       <c r="J182" s="21" t="s">
         <v>5</v>
@@ -11805,7 +11805,7 @@
         <v>B</v>
       </c>
       <c r="L182" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="M182" s="9">
         <v>1</v>

</xml_diff>

<commit_message>
chore: bump assets v=20251106_ 15606
Signed-off-by: nataliohoteles-crypto <comunicaciones@hotelguadiana.es>
</commit_message>
<xml_diff>
--- a/plantilla_preguntas_unica.xlsx
+++ b/plantilla_preguntas_unica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comun\Documents\Web Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DA2F58-EB2D-41E1-9A24-A51D2F4C3942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E02C1D4-F886-4B05-8C23-3FF0C1A43206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27840" yWindow="960" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Preguntas" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1810" uniqueCount="1031">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1810" uniqueCount="1032">
   <si>
     <t>id</t>
   </si>
@@ -3129,6 +3129,9 @@
   </si>
   <si>
     <t>Recepción</t>
+  </si>
+  <si>
+    <t>pisos</t>
   </si>
 </sst>
 </file>
@@ -4151,8 +4154,8 @@
   <dimension ref="A1:M182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A181" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D188" sqref="D188"/>
+      <pane ySplit="1" topLeftCell="A174" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B183" sqref="B183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11732,7 +11735,7 @@
         <v>180</v>
       </c>
       <c r="B181" s="18" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="C181" s="5" t="s">
         <v>1029</v>
@@ -11774,7 +11777,7 @@
         <v>181</v>
       </c>
       <c r="B182" s="18" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="C182" s="5" t="s">
         <v>1029</v>

</xml_diff>